<commit_message>
updated IO files and RTMF
</commit_message>
<xml_diff>
--- a/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
+++ b/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\trans\RTMF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\trans\RTMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879C9A3C-65AE-46B7-AAAF-3BEC51FB4A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D2FF57-3CF1-4CD4-9938-3F81DC6CC47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12870" yWindow="1470" windowWidth="22500" windowHeight="21135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="190" yWindow="100" windowWidth="12270" windowHeight="10140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -532,19 +532,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -552,80 +552,80 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>24</v>
@@ -634,7 +634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>25</v>
@@ -643,7 +643,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>26</v>
@@ -665,16 +665,18 @@
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -700,7 +702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -708,13 +710,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="4">
-        <v>0.33</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
       </c>
       <c r="E2" s="4">
-        <v>0.33</v>
+        <v>0.11</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
@@ -725,10 +727,10 @@
       <c r="H2" s="4"/>
       <c r="I2" s="6">
         <f>1-SUM(B2:G2)</f>
-        <v>0.33999999999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.32999999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -756,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -784,7 +786,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -812,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -840,7 +842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -868,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -891,14 +893,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -924,7 +926,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -952,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -980,7 +982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1008,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1036,7 +1038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1064,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1092,7 +1094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>

</xml_diff>